<commit_message>
Version 1~15 comments updated
</commit_message>
<xml_diff>
--- a/Sitecore Pilot Reflection - Updated.xlsx
+++ b/Sitecore Pilot Reflection - Updated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="25680" yWindow="420" windowWidth="20715" windowHeight="12330"/>
+    <workbookView xWindow="25680" yWindow="420" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="136">
   <si>
     <t>Category</t>
   </si>
@@ -118,9 +118,6 @@
     <t>There is only one staging environment on the Group Sitecore instance and there was some pressure from Group to get our website out of the staging environment as to not affect the Group project work that was in progress. We were not aware of the fact that there was only one staging environment.</t>
   </si>
   <si>
-    <t>Scheduling and communication is important however having more than one environment would certainty mitigate this.</t>
-  </si>
-  <si>
     <t>HTC's Client Relationship Management</t>
   </si>
   <si>
@@ -386,13 +383,109 @@
   </si>
   <si>
     <t>Developers on this project expressed concerns with the way they were being managed by JLTi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scheduling and communication is important however having more than one environment would certainty mitigate this.
+</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This code review process is in-place as the source code is common for Group sites and BSA. Since the code is developed by vendor and they mayn't be aware of impacts while making the changes in the existing code. Also after deployment the application support resides with JLT (not vendor). So code review is very important practise before accepting the code from vendor. 
+Going forward this need be enforced as process and included in the project plan.
+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In general every websites/application, undergo the PEN test before go-live in the security aspects. This may get tailored based on the project.
+Going forward this needs to be discussed/reviewed with Group/security Architect and include in the project/integration plan scope. 
+Additionally If any AU specific security guideline also may be considered.
+Also Security Group architect can provide the application web security check-list to adhere/review before PEN test.
+</t>
+  </si>
+  <si>
+    <t>Same as above</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This concerns can be addressed in two ways
+1. Project kick-off meeting and discussion with Group PM/architect
+2. Publish or Review Group Project Process in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>internal Wiki?</t>
+    </r>
+  </si>
+  <si>
+    <t>This is again lack of integration or deployment plan. If we have the deployment plan in-place this will be covered</t>
+  </si>
+  <si>
+    <t>This is infrastructure access is security requirement, all the servers is not accessible/across across all the regional IT location and vendor.
+This environmnet access has to be part of Project Initiation activities. Which includes
+Development tools purchase/access, connectivity establishment, environment access and development practise kt and etc..</t>
+  </si>
+  <si>
+    <t>This delay is not due to log access. Sravani reviewed the code and there is no log enabled for troubleshooting. After that JLTi requested vendor to include troubleshooting log and code deployed to UAT for troubleshooting.
+Addtionally UAT environment and log access in restricted as a infra security requirement. This is applicable irrespective of sitecore/non-sitecore applications for everyone. In the JLTi perspective we have provided the UAT log as soon its being requested as this critical input for troubleshooting.
+Sitecore development cost is not expensive compare with other tools/application for the Web CMS features used in BSA sites. We have such flexibility in web CMS compare with other options and development team should understand and implement properly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This helix principles introduced in 2016-Jan to support the Sitecore MVC architecture styles.
+This sitecore application being developed using sitecore 7.2 in 2014. During this time Sitecore webforms and component architecture supported in sitecore 7.2. Since then no architectural changes/migration implemented.
+This is one of the mandatory application architecture changes/upgrade required. Sitecore also reviewed and advised to to upgrade to Helix principles
+</t>
+  </si>
+  <si>
+    <t>Since we have sitecore license limitations/stage environment is sharable across all the sites. So the impact might be raised by group team.
+This can be mitigated in two ways.
+1. Group Project and Australia project PM's create the integrated project plan in the aspects of deployment timelines without conflicts.
+2. Revist the sitecore licensing model (consumption based) and introduce the seperate environment for AU sites.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As we understand this BSA site integration with group sites should be known in the beginning itself. If so there should be a discussion with group PM to understand the group project process and integration task.
+Going forward if we include the group project integration plan which covers the development practise, code review, testing activities like integration, regression, PEN,  performance testing and deployment with RACI and timelines.
+</t>
+  </si>
+  <si>
+    <t>This is again missing of integration plan. If we have that in-place we should be able to handle better.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vendor not communicated to JLTi that BSA new code changes using the new cookie. It took some time to identify the issue and communicated ensono to whitelist the cookies from security aspects.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">As we understand this BSA application integration and deployment not known/communicated to infra. architect and ensono (vendor). </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Still JLTi and Infra architect supported during vacation to fast track and troubleshoot this issue in the production. 
+As part of integration deployment plan if we include deployment support/ownership from group/ensono team, we get the people in-place well advance.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -412,8 +505,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -444,8 +549,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -468,11 +579,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -494,6 +625,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -796,24 +942,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1328125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="29.59765625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="44.73046875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="15.59765625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="30.86328125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="40.1328125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="29.6328125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="44.7265625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="30.81640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="40.08984375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="54.54296875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -832,8 +979,11 @@
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G1" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -844,16 +994,19 @@
         <v>32</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -861,19 +1014,22 @@
         <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="131.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -881,19 +1037,22 @@
         <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -901,19 +1060,22 @@
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -921,19 +1083,22 @@
         <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="23" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -941,19 +1106,22 @@
         <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="23" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -961,19 +1129,22 @@
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="50" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -981,19 +1152,22 @@
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="34.9" x14ac:dyDescent="0.35">
+      <c r="G9" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1001,19 +1175,22 @@
         <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="34.9" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="126.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1021,19 +1198,22 @@
         <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1041,139 +1221,154 @@
         <v>29</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="34.9" x14ac:dyDescent="0.35">
+      <c r="G12" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="100" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="34.9" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="200" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="G15" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="46" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="58.15" x14ac:dyDescent="0.35">
+      <c r="G16" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="57.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="34.9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="104.65" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="103.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
@@ -1181,161 +1376,161 @@
         <v>12</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="46" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:6" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="80.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C22" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="2" t="s">
+    </row>
+    <row r="23" spans="1:6" ht="46" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="69" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="57.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="58.15" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="58.15" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="34.9" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>5</v>
@@ -1343,66 +1538,66 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:6" ht="34.9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C28" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>104</v>
-      </c>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>108</v>
-      </c>
       <c r="D29" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="46" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="D30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="69.75" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:6" ht="69" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>31</v>
@@ -1411,13 +1606,13 @@
         <v>5</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="69.75" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:6" ht="69" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>3</v>
       </c>
@@ -1425,19 +1620,19 @@
         <v>13</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="58.15" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="57.5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>3</v>
       </c>
@@ -1445,19 +1640,19 @@
         <v>22</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="58.15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:6" ht="57.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
@@ -1465,19 +1660,19 @@
         <v>14</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="34.9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>3</v>
       </c>
@@ -1485,19 +1680,19 @@
         <v>15</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E35" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:6" ht="46" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>3</v>
       </c>
@@ -1505,16 +1700,16 @@
         <v>28</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E36" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>